<commit_message>
Updated Weather Station files
</commit_message>
<xml_diff>
--- a/Assembly_files/BOM_weather_station_PCB.xlsx
+++ b/Assembly_files/BOM_weather_station_PCB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diogoinacio/Documents/Gitlab/WS/Assembly_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3353DBF6-DC27-1444-9D5D-5538BC1E6E2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2499617-F847-EF4E-8906-63D43FAEEADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="84800" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{4E7C5F4B-8DB4-D84B-93D8-95D814A72D1A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{4E7C5F4B-8DB4-D84B-93D8-95D814A72D1A}"/>
   </bookViews>
   <sheets>
     <sheet name="pcb WS" sheetId="5" r:id="rId1"/>
@@ -26,7 +26,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="182">
   <si>
     <t>0ZCK0075FF2E</t>
   </si>
@@ -186,9 +190,6 @@
     <t>CN1</t>
   </si>
   <si>
-    <t>S2B-PH-SM4-TB</t>
-  </si>
-  <si>
     <t>SI2333DDS-T1-GE3</t>
   </si>
   <si>
@@ -216,9 +217,6 @@
     <t>R11 R12</t>
   </si>
   <si>
-    <t>C1 C2</t>
-  </si>
-  <si>
     <t>R29</t>
   </si>
   <si>
@@ -238,9 +236,6 @@
   </si>
   <si>
     <t>RC0603FR-132K74L</t>
-  </si>
-  <si>
-    <t>C4 C9</t>
   </si>
   <si>
     <t>R9 R24</t>
@@ -347,13 +342,7 @@
     <t>Taiwan Semiconductor</t>
   </si>
   <si>
-    <t>R14 R15 R26</t>
-  </si>
-  <si>
     <t>R23 R25 R36</t>
-  </si>
-  <si>
-    <t>Q1 Q3 Q9</t>
   </si>
   <si>
     <t>C5 C6 C7 C10</t>
@@ -432,9 +421,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Cathode has a mark (".")</t>
-  </si>
-  <si>
     <t>RES Thick Film Resistors - SMD 0603 1K 1% 1/10W</t>
   </si>
   <si>
@@ -536,26 +522,14 @@
     <t>Ethernet Connectors RA 6/6 RJ12 LOW PROFILE THT</t>
   </si>
   <si>
-    <t xml:space="preserve">D1 D2 D4 D5 D6 D7 D8 </t>
-  </si>
-  <si>
     <t>D11
 Or
 D9</t>
   </si>
   <si>
-    <t xml:space="preserve">If has problem to buy the  D11 item, can you buy the D9 item   </t>
-  </si>
-  <si>
     <t>Green_LED</t>
   </si>
   <si>
-    <t>R16 R37</t>
-  </si>
-  <si>
-    <t>R16 &amp; R37: Soldering RES jumper (or Shunt)</t>
-  </si>
-  <si>
     <t>JP5</t>
   </si>
   <si>
@@ -575,13 +549,63 @@
   </si>
   <si>
     <t>22k</t>
+  </si>
+  <si>
+    <t>Alternative: EBBA-02-C-SS-BU</t>
+  </si>
+  <si>
+    <t>Alternative: C0805C475K4RACAUTO</t>
+  </si>
+  <si>
+    <t>D1 D2 D4 D5 D6 D7 D8 D12</t>
+  </si>
+  <si>
+    <t>Alternative: DMG2305UX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alternative: 54601-906WPLF </t>
+  </si>
+  <si>
+    <t>S2B-PH-SM4-TB(LF)(SN)</t>
+  </si>
+  <si>
+    <t>Cathode has a mark (".")
+Alternative: LTST-C170KGKT</t>
+  </si>
+  <si>
+    <t>Alternative: KDV08FR200ET</t>
+  </si>
+  <si>
+    <t>C1 C2</t>
+  </si>
+  <si>
+    <t>Q1 Q3 Q9</t>
+  </si>
+  <si>
+    <t>R16 R37 R40</t>
+  </si>
+  <si>
+    <t>Soldering RES jumper (or Shunt)</t>
+  </si>
+  <si>
+    <t>Alternative: B2B-PH-SM4-TB (pins aligned to the outside of the board)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If has problem to buy the D11 item, can you buy the D9 item
+D11 Alternative: SMBJ5339B-TP   </t>
+  </si>
+  <si>
+    <t>R14 R15 R26 R39</t>
+  </si>
+  <si>
+    <t>C4 C9 C13</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -691,7 +715,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -768,6 +792,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1082,58 +1109,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF8389C6-3F49-704F-94B7-39ACBC3F2AF1}">
-  <dimension ref="A1:R37"/>
+  <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="158" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="10.1640625" customWidth="1"/>
-    <col min="3" max="3" width="5.33203125" customWidth="1"/>
-    <col min="4" max="4" width="8" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" customWidth="1"/>
-    <col min="7" max="7" width="11.5" style="5" customWidth="1"/>
-    <col min="8" max="8" width="33.33203125" customWidth="1"/>
-    <col min="9" max="9" width="5.6640625" customWidth="1"/>
-    <col min="10" max="10" width="12" style="10" customWidth="1"/>
+    <col min="1" max="1" width="7.5" style="6" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" style="10" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="4" customFormat="1" ht="51">
+    <row r="1" spans="1:18" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D1" s="26" t="s">
         <v>7</v>
       </c>
       <c r="E1" s="27" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="F1" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="G1" s="27" t="s">
-        <v>74</v>
-      </c>
       <c r="H1" s="26" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I1" s="28" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="J1" s="26" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
@@ -1144,33 +1171,33 @@
       <c r="Q1" s="3"/>
       <c r="R1" s="3"/>
     </row>
-    <row r="2" spans="1:18" ht="30">
+    <row r="2" spans="1:18" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" s="12">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" s="13">
+      <c r="B2" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="C2" s="20">
         <v>2</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>18</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F2" s="14" t="s">
         <v>19</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="J2" s="16"/>
       <c r="K2" s="1"/>
@@ -1182,7 +1209,7 @@
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
     </row>
-    <row r="3" spans="1:18" ht="30">
+    <row r="3" spans="1:18" ht="30" x14ac:dyDescent="0.2">
       <c r="A3" s="12">
         <v>2</v>
       </c>
@@ -1196,19 +1223,19 @@
         <v>28</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F3" s="13" t="s">
         <v>30</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="J3" s="17"/>
       <c r="K3" s="1"/>
@@ -1220,33 +1247,33 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:18" ht="30">
+    <row r="4" spans="1:18" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="12">
         <v>3</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="C4" s="13">
-        <v>2</v>
+      <c r="B4" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="C4" s="20">
+        <v>3</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F4" s="13" t="s">
         <v>14</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H4" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="I4" s="15" t="s">
         <v>118</v>
-      </c>
-      <c r="I4" s="15" t="s">
-        <v>123</v>
       </c>
       <c r="J4" s="18"/>
       <c r="K4" s="1"/>
@@ -1258,12 +1285,12 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="12">
         <v>4</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C5" s="13">
         <v>4</v>
@@ -1272,19 +1299,19 @@
         <v>21</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="F5" s="13" t="s">
         <v>22</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="J5" s="19"/>
       <c r="K5" s="1"/>
@@ -1296,7 +1323,7 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
     </row>
-    <row r="6" spans="1:18" ht="30">
+    <row r="6" spans="1:18" ht="45" x14ac:dyDescent="0.2">
       <c r="A6" s="12">
         <v>5</v>
       </c>
@@ -1310,21 +1337,23 @@
         <v>37</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>39</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="I6" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="J6" s="17"/>
+        <v>118</v>
+      </c>
+      <c r="J6" s="22" t="s">
+        <v>167</v>
+      </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="2"/>
@@ -1334,7 +1363,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" ht="30">
+    <row r="7" spans="1:18" ht="60" x14ac:dyDescent="0.2">
       <c r="A7" s="12">
         <v>6</v>
       </c>
@@ -1351,18 +1380,20 @@
         <v>48</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>50</v>
+        <v>171</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="J7" s="17"/>
+        <v>118</v>
+      </c>
+      <c r="J7" s="30" t="s">
+        <v>178</v>
+      </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -1372,33 +1403,33 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
     </row>
-    <row r="8" spans="1:18" ht="30">
+    <row r="8" spans="1:18" ht="30" x14ac:dyDescent="0.2">
       <c r="A8" s="12">
         <v>7</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>163</v>
-      </c>
-      <c r="C8" s="13">
-        <v>7</v>
+        <v>168</v>
+      </c>
+      <c r="C8" s="20">
+        <v>8</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="I8" s="15" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="J8" s="17"/>
       <c r="K8" s="1"/>
@@ -1410,36 +1441,36 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
     </row>
-    <row r="9" spans="1:18" ht="105">
+    <row r="9" spans="1:18" ht="105" x14ac:dyDescent="0.2">
       <c r="A9" s="12">
         <v>8</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="C9" s="21">
         <v>1</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>165</v>
+        <v>179</v>
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
@@ -1450,33 +1481,33 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
     </row>
-    <row r="10" spans="1:18" ht="30">
+    <row r="10" spans="1:18" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" s="12">
         <v>9</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C10" s="21">
         <v>2</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="I10" s="15" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="J10" s="17"/>
       <c r="K10" s="1"/>
@@ -1488,12 +1519,12 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
     </row>
-    <row r="11" spans="1:18" ht="30">
+    <row r="11" spans="1:18" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" s="12">
         <v>10</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C11" s="13">
         <v>2</v>
@@ -1508,13 +1539,13 @@
         <v>0</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="I11" s="15" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="J11" s="17"/>
       <c r="K11" s="1"/>
@@ -1526,12 +1557,12 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
     </row>
-    <row r="12" spans="1:18" ht="30">
+    <row r="12" spans="1:18" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="12">
         <v>11</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C12" s="13">
         <v>2</v>
@@ -1546,15 +1577,17 @@
         <v>47</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="J12" s="17"/>
+        <v>121</v>
+      </c>
+      <c r="J12" s="22" t="s">
+        <v>170</v>
+      </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
@@ -1564,33 +1597,33 @@
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
     </row>
-    <row r="13" spans="1:18" ht="30">
+    <row r="13" spans="1:18" ht="30" x14ac:dyDescent="0.2">
       <c r="A13" s="12">
         <v>12</v>
       </c>
-      <c r="B13" s="13" t="s">
-        <v>157</v>
+      <c r="B13" s="20" t="s">
+        <v>151</v>
       </c>
       <c r="C13" s="13">
         <v>2</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="E13" s="13" t="s">
         <v>42</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="J13" s="17"/>
       <c r="K13" s="1"/>
@@ -1602,33 +1635,33 @@
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
     </row>
-    <row r="14" spans="1:18" ht="30">
+    <row r="14" spans="1:18" ht="30" x14ac:dyDescent="0.2">
       <c r="A14" s="12">
         <v>13</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="C14" s="13">
         <v>1</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="I14" s="15" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="J14" s="17"/>
       <c r="K14" s="1"/>
@@ -1640,35 +1673,37 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:18" ht="30">
+    <row r="15" spans="1:18" ht="30" x14ac:dyDescent="0.2">
       <c r="A15" s="12">
         <v>14</v>
       </c>
-      <c r="B15" s="13" t="s">
-        <v>174</v>
+      <c r="B15" s="20" t="s">
+        <v>164</v>
       </c>
       <c r="C15" s="13">
         <v>4</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="E15" s="13" t="s">
         <v>12</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I15" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="J15" s="17"/>
+        <v>121</v>
+      </c>
+      <c r="J15" s="22" t="s">
+        <v>166</v>
+      </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
@@ -1678,7 +1713,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" ht="30">
+    <row r="16" spans="1:18" ht="60" x14ac:dyDescent="0.2">
       <c r="A16" s="12">
         <v>15</v>
       </c>
@@ -1689,25 +1724,25 @@
         <v>1</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F16" s="13" t="s">
         <v>9</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I16" s="15" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="J16" s="22" t="s">
-        <v>129</v>
+        <v>172</v>
       </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -1718,35 +1753,37 @@
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
     </row>
-    <row r="17" spans="1:18" ht="30">
+    <row r="17" spans="1:18" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" s="12">
         <v>16</v>
       </c>
-      <c r="B17" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="C17" s="13">
+      <c r="B17" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="C17" s="20">
         <v>3</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="I17" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="J17" s="17"/>
+        <v>118</v>
+      </c>
+      <c r="J17" s="22" t="s">
+        <v>169</v>
+      </c>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
@@ -1756,12 +1793,12 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
     </row>
-    <row r="18" spans="1:18" ht="30">
+    <row r="18" spans="1:18" ht="30" x14ac:dyDescent="0.2">
       <c r="A18" s="12">
         <v>17</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C18" s="13">
         <v>3</v>
@@ -1770,19 +1807,19 @@
         <v>40</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="F18" s="13" t="s">
         <v>3</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="J18" s="17"/>
       <c r="K18" s="1"/>
@@ -1794,7 +1831,7 @@
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
     </row>
-    <row r="19" spans="1:18" ht="45">
+    <row r="19" spans="1:18" ht="45" x14ac:dyDescent="0.2">
       <c r="A19" s="12">
         <v>18</v>
       </c>
@@ -1808,19 +1845,19 @@
         <v>6</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="I19" s="15" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="J19" s="17"/>
       <c r="K19" s="1"/>
@@ -1832,7 +1869,7 @@
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
     </row>
-    <row r="20" spans="1:18" ht="30">
+    <row r="20" spans="1:18" ht="30" x14ac:dyDescent="0.2">
       <c r="A20" s="12">
         <v>19</v>
       </c>
@@ -1846,21 +1883,23 @@
         <v>25</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="F20" s="13" t="s">
         <v>27</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="I20" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="J20" s="17"/>
+        <v>118</v>
+      </c>
+      <c r="J20" s="22" t="s">
+        <v>173</v>
+      </c>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
@@ -1870,12 +1909,12 @@
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
     </row>
-    <row r="21" spans="1:18" ht="30">
+    <row r="21" spans="1:18" ht="30" x14ac:dyDescent="0.2">
       <c r="A21" s="12">
         <v>20</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C21" s="13">
         <v>2</v>
@@ -1884,19 +1923,19 @@
         <v>15</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F21" s="13" t="s">
         <v>16</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="J21" s="17"/>
       <c r="K21" s="1"/>
@@ -1908,12 +1947,12 @@
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
     </row>
-    <row r="22" spans="1:18" ht="30">
+    <row r="22" spans="1:18" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" s="12">
         <v>21</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C22" s="13">
         <v>4</v>
@@ -1922,49 +1961,49 @@
         <v>31</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F22" s="13" t="s">
         <v>32</v>
       </c>
       <c r="G22" s="15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H22" s="13" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="I22" s="15" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="J22" s="17"/>
     </row>
-    <row r="23" spans="1:18" ht="30">
+    <row r="23" spans="1:18" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" s="12">
         <v>22</v>
       </c>
-      <c r="B23" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="C23" s="13">
-        <v>3</v>
+      <c r="B23" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="C23" s="20">
+        <v>4</v>
       </c>
       <c r="D23" s="13" t="s">
         <v>4</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F23" s="13" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="I23" s="15" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="J23" s="29"/>
       <c r="K23" s="1"/>
@@ -1976,36 +2015,36 @@
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
     </row>
-    <row r="24" spans="1:18" ht="60">
+    <row r="24" spans="1:18" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" s="12">
         <v>23</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="C24" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F24" s="13" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="G24" s="21" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="I24" s="15" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="J24" s="13" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -2016,12 +2055,12 @@
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
     </row>
-    <row r="25" spans="1:18" ht="30">
+    <row r="25" spans="1:18" ht="30" x14ac:dyDescent="0.2">
       <c r="A25" s="12">
         <v>24</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C25" s="13">
         <v>3</v>
@@ -2030,19 +2069,19 @@
         <v>5</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F25" s="13" t="s">
         <v>13</v>
       </c>
       <c r="G25" s="15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="I25" s="15" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="J25" s="17"/>
       <c r="K25" s="1"/>
@@ -2054,12 +2093,12 @@
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
     </row>
-    <row r="26" spans="1:18" ht="30">
+    <row r="26" spans="1:18" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" s="12">
         <v>25</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C26" s="13">
         <v>3</v>
@@ -2068,49 +2107,49 @@
         <v>23</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F26" s="13" t="s">
         <v>24</v>
       </c>
       <c r="G26" s="15" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="I26" s="15" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="J26" s="17"/>
     </row>
-    <row r="27" spans="1:18" ht="30">
+    <row r="27" spans="1:18" ht="30" x14ac:dyDescent="0.2">
       <c r="A27" s="12">
         <v>26</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C27" s="13">
         <v>1</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F27" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G27" s="15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H27" s="13" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="I27" s="15" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="J27" s="17"/>
       <c r="K27" s="1"/>
@@ -2122,7 +2161,7 @@
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
     </row>
-    <row r="28" spans="1:18" ht="30">
+    <row r="28" spans="1:18" ht="30" x14ac:dyDescent="0.2">
       <c r="A28" s="12">
         <v>27</v>
       </c>
@@ -2136,19 +2175,19 @@
         <v>35</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F28" s="13" t="s">
         <v>17</v>
       </c>
       <c r="G28" s="15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="I28" s="15" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="J28" s="17"/>
       <c r="K28" s="1"/>
@@ -2160,7 +2199,7 @@
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
     </row>
-    <row r="29" spans="1:18" ht="30">
+    <row r="29" spans="1:18" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" s="12">
         <v>28</v>
       </c>
@@ -2171,22 +2210,22 @@
         <v>1</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F29" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G29" s="15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="I29" s="15" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="J29" s="17"/>
       <c r="K29" s="1"/>
@@ -2198,12 +2237,12 @@
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
     </row>
-    <row r="30" spans="1:18" ht="30">
+    <row r="30" spans="1:18" ht="30" x14ac:dyDescent="0.2">
       <c r="A30" s="12">
         <v>29</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C30" s="13">
         <v>2</v>
@@ -2212,23 +2251,23 @@
         <v>33</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F30" s="13" t="s">
         <v>34</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H30" s="15" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="I30" s="15" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="J30" s="17"/>
     </row>
-    <row r="31" spans="1:18" ht="30">
+    <row r="31" spans="1:18" ht="30" x14ac:dyDescent="0.2">
       <c r="A31" s="12">
         <v>30</v>
       </c>
@@ -2239,22 +2278,22 @@
         <v>1</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="E31" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="G31" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="H31" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="F31" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="G31" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="H31" s="13" t="s">
-        <v>148</v>
-      </c>
       <c r="I31" s="15" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="J31" s="17"/>
       <c r="K31" s="1"/>
@@ -2266,7 +2305,7 @@
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
     </row>
-    <row r="32" spans="1:18" ht="30">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" s="12">
         <v>31</v>
       </c>
@@ -2277,56 +2316,56 @@
         <v>1</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F32" s="13" t="s">
         <v>11</v>
       </c>
       <c r="G32" s="15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H32" s="13" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="I32" s="15" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="J32" s="24"/>
     </row>
-    <row r="33" spans="1:10" ht="45">
+    <row r="33" spans="1:10" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="12">
         <v>32</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C33" s="21">
         <v>1</v>
       </c>
       <c r="D33" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="F33" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G33" s="15" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="I33" s="15" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="J33" s="29"/>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B34" s="8"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
@@ -2336,21 +2375,11 @@
       <c r="H34" s="8"/>
       <c r="I34" s="9"/>
     </row>
-    <row r="35" spans="1:10">
-      <c r="B35" s="8"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="9"/>
-    </row>
-    <row r="36" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G35" s="10"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G36" s="10"/>
-    </row>
-    <row r="37" spans="1:10">
-      <c r="G37" s="10"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J32" xr:uid="{1CE811C6-D828-E044-BA15-354C3D8A2352}">
@@ -2364,15 +2393,10 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E4BBE1C408CB0C41B84CADD8BCFCE7E9" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7016465824c282551da233d50adaebaa">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a34c0613-ef4b-4602-8030-b44b96bc6f4f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e3755edb0548f2a2eee8e81050632832" ns2:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E4BBE1C408CB0C41B84CADD8BCFCE7E9" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4cb08661ca6b7b8f883b04a888ddde4e">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a34c0613-ef4b-4602-8030-b44b96bc6f4f" xmlns:ns3="d9decd26-93d6-4690-978f-3b51b4a374e2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="81b138b4a0b898bdcdf026d23b9d3dd3" ns2:_="" ns3:_="">
     <xsd:import namespace="a34c0613-ef4b-4602-8030-b44b96bc6f4f"/>
+    <xsd:import namespace="d9decd26-93d6-4690-978f-3b51b4a374e2"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
@@ -2383,6 +2407,16 @@
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -2414,6 +2448,86 @@
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="12" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="13" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="16" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="17" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="21" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="4d2ad2af-2f6f-4a43-825f-ce868cea6adf" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="d9decd26-93d6-4690-978f-3b51b4a374e2" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="18" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="19" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="22" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{8369bda3-54d8-4014-b870-bfd33711fa12}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="d9decd26-93d6-4690-978f-3b51b4a374e2">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
@@ -2515,7 +2629,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2524,30 +2638,26 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45E492BE-B035-4357-8A04-FBCF05117C95}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="a34c0613-ef4b-4602-8030-b44b96bc6f4f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="d9decd26-93d6-4690-978f-3b51b4a374e2" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a34c0613-ef4b-4602-8030-b44b96bc6f4f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90A06C95-84E0-4B46-8E6D-A92D8B7FAC16}">
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A5071EC-AAFA-42A9-A752-E2F3DF8623CF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="a34c0613-ef4b-4602-8030-b44b96bc6f4f"/>
+    <ds:schemaRef ds:uri="d9decd26-93d6-4690-978f-3b51b4a374e2"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -2558,10 +2668,27 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D7B7B8A-160B-4B96-9DD7-0ED039BD652C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45E492BE-B035-4357-8A04-FBCF05117C95}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="a34c0613-ef4b-4602-8030-b44b96bc6f4f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d9decd26-93d6-4690-978f-3b51b4a374e2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>